<commit_message>
Atualização documentação Conferência - LN
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_DOM.xlsx
+++ b/Documentação/Planilhas/Conferencia_DOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" firstSheet="65" activeTab="70"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="93" r:id="rId1"/>
@@ -84,7 +84,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2889" uniqueCount="1582">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2895" uniqueCount="1587">
   <si>
     <t>DESCR</t>
   </si>
@@ -4875,12 +4875,31 @@
   <si>
     <t>Dado do WMS</t>
   </si>
+  <si>
+    <t>Sessão tfgld0510m000</t>
+  </si>
+  <si>
+    <t>sessão tcemm0130m000 [usar o CD_Filial identificado na sessão tfgld0510m000 como chave]</t>
+  </si>
+  <si>
+    <t>Fixo como 201</t>
+  </si>
+  <si>
+    <t>Selecionar a Unidade Empresarial referente ao CD_FILIAL desejado
+Ir no menu Referências e escolher "Parceiro de Negócio Interno"
+Na aba Geral, pedir o detalhamento do código do endereço
+Na aba Detalhado, seção Identificação de Imposto, pegar a informação da Entidade Fiscal 
+[na extração tem um tratamento para eliminar a "/" e o "-']</t>
+  </si>
+  <si>
+    <t>tfgld0510m000, tcemm0130m000 e tccom0502m000</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="12">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4969,6 +4988,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="10">
     <fill>
@@ -5026,7 +5052,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="21">
     <border>
       <left/>
       <right/>
@@ -5256,6 +5282,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -5264,7 +5316,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="122">
+  <cellXfs count="125">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -5523,17 +5575,17 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -5544,28 +5596,28 @@
     <xf numFmtId="49" fontId="7" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="7" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="7" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="7" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5593,6 +5645,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7000,11 +7061,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
+      <selection pane="bottomRight" activeCell="B73" sqref="B73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14337,10 +14398,10 @@
       <c r="AF5" s="2"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1014</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="D6" s="36" t="s">
         <v>786</v>
       </c>
@@ -14462,10 +14523,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>710</v>
@@ -14473,21 +14534,21 @@
       <c r="E19" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="100" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="99"/>
+      <c r="F20" s="101"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:6">
@@ -14504,10 +14565,10 @@
       <c r="F23" s="48"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="98" t="s">
         <v>1016</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="98"/>
       <c r="D25" s="36" t="s">
         <v>786</v>
       </c>
@@ -14629,10 +14690,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="99"/>
       <c r="C38" s="46"/>
       <c r="D38" s="68" t="s">
         <v>710</v>
@@ -14640,21 +14701,21 @@
       <c r="E38" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F38" s="98" t="s">
+      <c r="F38" s="100" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="99"/>
+      <c r="B39" s="99"/>
       <c r="C39" s="46"/>
       <c r="D39" s="68"/>
       <c r="E39" s="68"/>
-      <c r="F39" s="99"/>
+      <c r="F39" s="101"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="46"/>
     </row>
     <row r="41" spans="1:6">
@@ -14664,11 +14725,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A38:B40"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="A2:B2"/>
@@ -14676,6 +14732,11 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A19:B21"/>
     <mergeCell ref="D19:D20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A38:B40"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -15026,11 +15087,6 @@
     </row>
   </sheetData>
   <mergeCells count="12">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="D42:E42"/>
     <mergeCell ref="D49:E49"/>
     <mergeCell ref="D43:E43"/>
     <mergeCell ref="D44:E44"/>
@@ -15038,6 +15094,11 @@
     <mergeCell ref="D46:E46"/>
     <mergeCell ref="D47:E47"/>
     <mergeCell ref="D48:E48"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="D42:E42"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -17158,17 +17219,17 @@
       <c r="A19" s="104" t="s">
         <v>916</v>
       </c>
-      <c r="B19" s="110"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="107"/>
+      <c r="B19" s="105"/>
+      <c r="C19" s="105"/>
+      <c r="D19" s="105"/>
+      <c r="E19" s="105"/>
+      <c r="F19" s="105"/>
+      <c r="G19" s="105"/>
+      <c r="H19" s="106"/>
       <c r="I19" s="104" t="s">
         <v>917</v>
       </c>
-      <c r="J19" s="107"/>
+      <c r="J19" s="106"/>
       <c r="K19" s="104" t="s">
         <v>920</v>
       </c>
@@ -17176,32 +17237,32 @@
       <c r="M19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="11.25" customHeight="1">
-      <c r="A20" s="105"/>
-      <c r="B20" s="111"/>
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="108"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="105"/>
+      <c r="A20" s="107"/>
+      <c r="B20" s="108"/>
+      <c r="C20" s="108"/>
+      <c r="D20" s="108"/>
+      <c r="E20" s="108"/>
+      <c r="F20" s="108"/>
+      <c r="G20" s="108"/>
+      <c r="H20" s="109"/>
+      <c r="I20" s="107"/>
+      <c r="J20" s="109"/>
+      <c r="K20" s="107"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="106"/>
-      <c r="B21" s="112"/>
-      <c r="C21" s="112"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="112"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="106"/>
-      <c r="J21" s="109"/>
-      <c r="K21" s="106"/>
+      <c r="A21" s="110"/>
+      <c r="B21" s="111"/>
+      <c r="C21" s="111"/>
+      <c r="D21" s="111"/>
+      <c r="E21" s="111"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="111"/>
+      <c r="H21" s="112"/>
+      <c r="I21" s="110"/>
+      <c r="J21" s="112"/>
+      <c r="K21" s="110"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
     </row>
@@ -17442,22 +17503,22 @@
     </row>
   </sheetData>
   <mergeCells count="16">
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="B22:B25"/>
-    <mergeCell ref="A22:A25"/>
-    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="K19:K21"/>
+    <mergeCell ref="K22:K25"/>
+    <mergeCell ref="I19:J21"/>
+    <mergeCell ref="I22:I25"/>
+    <mergeCell ref="J22:J25"/>
     <mergeCell ref="H22:H25"/>
     <mergeCell ref="A19:H21"/>
     <mergeCell ref="F22:F25"/>
     <mergeCell ref="G22:G25"/>
     <mergeCell ref="D22:D25"/>
     <mergeCell ref="E22:E25"/>
-    <mergeCell ref="K19:K21"/>
-    <mergeCell ref="K22:K25"/>
-    <mergeCell ref="I19:J21"/>
-    <mergeCell ref="I22:I25"/>
-    <mergeCell ref="J22:J25"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="B22:B25"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="C22:C25"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -18517,6 +18578,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="G22:G25"/>
+    <mergeCell ref="H22:H25"/>
+    <mergeCell ref="E22:E25"/>
+    <mergeCell ref="F22:F25"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
     <mergeCell ref="P22:P25"/>
     <mergeCell ref="Q22:Q25"/>
     <mergeCell ref="A19:C21"/>
@@ -18533,12 +18600,6 @@
     <mergeCell ref="B22:B25"/>
     <mergeCell ref="D19:D21"/>
     <mergeCell ref="D22:D25"/>
-    <mergeCell ref="G22:G25"/>
-    <mergeCell ref="H22:H25"/>
-    <mergeCell ref="E22:E25"/>
-    <mergeCell ref="F22:F25"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -21460,10 +21521,10 @@
       <c r="AF5" s="2"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1120</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="D6" s="36" t="s">
         <v>1116</v>
       </c>
@@ -21562,30 +21623,30 @@
       <c r="E15" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F15" s="98" t="s">
+      <c r="F15" s="100" t="s">
         <v>1122</v>
       </c>
     </row>
     <row r="16" spans="1:32">
       <c r="D16" s="68"/>
       <c r="E16" s="68"/>
-      <c r="F16" s="99"/>
+      <c r="F16" s="101"/>
     </row>
     <row r="19" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:6">
@@ -21602,10 +21663,10 @@
       <c r="F23" s="48"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="98" t="s">
         <v>1121</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="98"/>
       <c r="D25" s="36" t="s">
         <v>1116</v>
       </c>
@@ -21711,30 +21772,30 @@
       <c r="E36" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F36" s="98" t="s">
+      <c r="F36" s="100" t="s">
         <v>1123</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="D37" s="68"/>
       <c r="E37" s="68"/>
-      <c r="F37" s="99"/>
+      <c r="F37" s="101"/>
     </row>
     <row r="38" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="99"/>
       <c r="C38" s="46"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="99"/>
+      <c r="B39" s="99"/>
       <c r="C39" s="46"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="46"/>
     </row>
     <row r="41" spans="1:6">
@@ -21744,6 +21805,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A19:B21"/>
+    <mergeCell ref="D15:D16"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="A38:B40"/>
@@ -21751,11 +21817,6 @@
     <mergeCell ref="E36:E37"/>
     <mergeCell ref="F36:F37"/>
     <mergeCell ref="E15:E16"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A19:B21"/>
-    <mergeCell ref="D15:D16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -21851,10 +21912,10 @@
       <c r="AF5" s="2"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1125</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="D6" s="36" t="s">
         <v>1129</v>
       </c>
@@ -21954,10 +22015,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>710</v>
@@ -21965,21 +22026,21 @@
       <c r="E19" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="100" t="s">
         <v>1126</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="99"/>
+      <c r="F20" s="101"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:6">
@@ -21996,10 +22057,10 @@
       <c r="F23" s="48"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="98" t="s">
         <v>1127</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="98"/>
       <c r="D25" s="36" t="s">
         <v>1129</v>
       </c>
@@ -22110,10 +22171,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="99"/>
       <c r="C38" s="46"/>
       <c r="D38" s="68" t="s">
         <v>710</v>
@@ -22121,21 +22182,21 @@
       <c r="E38" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F38" s="98" t="s">
+      <c r="F38" s="100" t="s">
         <v>1128</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="99"/>
+      <c r="B39" s="99"/>
       <c r="C39" s="46"/>
       <c r="D39" s="68"/>
       <c r="E39" s="68"/>
-      <c r="F39" s="99"/>
+      <c r="F39" s="101"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="46"/>
     </row>
     <row r="41" spans="1:6">
@@ -22145,18 +22206,18 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="A19:B21"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="A25:B25"/>
     <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="A38:B40"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="A19:B21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -22232,10 +22293,10 @@
       <c r="L3" s="13"/>
     </row>
     <row r="6" spans="1:33">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1140</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="36" t="s">
         <v>1137</v>
@@ -22411,10 +22472,10 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>710</v>
@@ -22422,23 +22483,23 @@
       <c r="E19" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="100" t="s">
         <v>1139</v>
       </c>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="99"/>
+      <c r="F20" s="101"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -22473,10 +22534,10 @@
       <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="98" t="s">
         <v>1141</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="98"/>
       <c r="C25" s="14"/>
       <c r="D25" s="36" t="s">
         <v>1137</v>
@@ -22658,10 +22719,10 @@
       <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="99"/>
       <c r="C38" s="46"/>
       <c r="D38" s="68" t="s">
         <v>710</v>
@@ -22669,23 +22730,23 @@
       <c r="E38" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F38" s="98" t="s">
+      <c r="F38" s="100" t="s">
         <v>1142</v>
       </c>
       <c r="G38" s="13"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="99"/>
+      <c r="B39" s="99"/>
       <c r="C39" s="46"/>
       <c r="D39" s="68"/>
       <c r="E39" s="68"/>
-      <c r="F39" s="99"/>
+      <c r="F39" s="101"/>
       <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="46"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
@@ -22789,10 +22850,10 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1125</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="36" t="s">
         <v>1145</v>
@@ -22951,10 +23012,10 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>710</v>
@@ -22962,25 +23023,25 @@
       <c r="E19" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="100" t="s">
         <v>1126</v>
       </c>
       <c r="G19" s="13"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="99"/>
+      <c r="F20" s="101"/>
       <c r="G20" s="13"/>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -23019,10 +23080,10 @@
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="98" t="s">
         <v>1144</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="98"/>
       <c r="C25" s="14"/>
       <c r="D25" s="36" t="s">
         <v>1145</v>
@@ -23211,10 +23272,10 @@
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="99"/>
       <c r="C38" s="46"/>
       <c r="D38" s="68" t="s">
         <v>710</v>
@@ -23222,25 +23283,25 @@
       <c r="E38" s="68" t="s">
         <v>711</v>
       </c>
-      <c r="F38" s="98" t="s">
+      <c r="F38" s="100" t="s">
         <v>1143</v>
       </c>
       <c r="G38" s="13"/>
       <c r="L38" s="2"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="99"/>
+      <c r="B39" s="99"/>
       <c r="C39" s="46"/>
       <c r="D39" s="68"/>
       <c r="E39" s="68"/>
-      <c r="F39" s="99"/>
+      <c r="F39" s="101"/>
       <c r="G39" s="13"/>
       <c r="L39" s="2"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="99"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="46"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
@@ -23275,6 +23336,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A38:B40"/>
+    <mergeCell ref="D38:D39"/>
     <mergeCell ref="E38:E39"/>
     <mergeCell ref="F38:F39"/>
     <mergeCell ref="A19:B21"/>
@@ -23282,11 +23348,6 @@
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A38:B40"/>
-    <mergeCell ref="D38:D39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -23361,10 +23422,10 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1158</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="19" t="s">
         <v>484</v>
@@ -23523,10 +23584,10 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>1159</v>
@@ -23541,8 +23602,8 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
@@ -23551,8 +23612,8 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
@@ -23653,10 +23714,10 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1158</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="19" t="s">
         <v>1173</v>
@@ -23801,10 +23862,10 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>1184</v>
@@ -23816,8 +23877,8 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
@@ -23825,8 +23886,8 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
@@ -25198,10 +25259,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1158</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1262</v>
@@ -25357,10 +25418,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1066</v>
@@ -25372,8 +25433,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -25381,8 +25442,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -26116,10 +26177,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1158</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1305</v>
@@ -26279,10 +26340,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1066</v>
@@ -26294,8 +26355,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -26303,8 +26364,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -28835,10 +28896,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1158</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1382</v>
@@ -28998,10 +29059,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1066</v>
@@ -29013,8 +29074,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -29022,8 +29083,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -29440,10 +29501,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1158</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>643</v>
@@ -29603,10 +29664,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1066</v>
@@ -29618,8 +29679,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -29627,8 +29688,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -29723,10 +29784,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1158</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1405</v>
@@ -29886,10 +29947,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1066</v>
@@ -29901,8 +29962,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -29910,8 +29971,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -30006,10 +30067,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="98" t="s">
         <v>1158</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="98"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1417</v>
@@ -30137,10 +30198,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="99" t="s">
         <v>709</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1066</v>
@@ -30152,8 +30213,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -30161,8 +30222,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -31390,10 +31451,10 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A2:AA20"/>
+  <dimension ref="A2:AA32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
@@ -31401,9 +31462,11 @@
     <col min="1" max="1" width="18.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="19.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19" style="1" customWidth="1"/>
-    <col min="6" max="8" width="17.5703125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="36.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="28.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" style="1" customWidth="1"/>
     <col min="9" max="9" width="11" style="1" customWidth="1"/>
     <col min="10" max="10" width="12.42578125" style="1" customWidth="1"/>
     <col min="11" max="11" width="18.85546875" style="1" customWidth="1"/>
@@ -31443,7 +31506,7 @@
       <c r="C2" s="3" t="s">
         <v>1550</v>
       </c>
-      <c r="D2" s="2"/>
+      <c r="H2" s="2"/>
       <c r="N2" s="1"/>
       <c r="P2" s="1"/>
       <c r="AA2" s="1"/>
@@ -31454,9 +31517,9 @@
       </c>
       <c r="B3" s="64"/>
       <c r="C3" s="3" t="s">
-        <v>478</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>1586</v>
+      </c>
+      <c r="H3" s="2"/>
       <c r="N3" s="1"/>
       <c r="P3" s="1"/>
       <c r="AA3" s="1"/>
@@ -31466,8 +31529,8 @@
       <c r="B4" s="2"/>
       <c r="C4" s="6"/>
       <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="H4" s="6"/>
       <c r="K4" s="2"/>
       <c r="M4" s="2"/>
       <c r="N4" s="1"/>
@@ -31480,25 +31543,25 @@
         <v>1463</v>
       </c>
       <c r="B6" s="16" t="s">
+        <v>1465</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>552</v>
+      </c>
+      <c r="D6" s="15" t="s">
+        <v>649</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>484</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>485</v>
+      </c>
+      <c r="G6" s="16" t="s">
+        <v>1466</v>
+      </c>
+      <c r="H6" s="16" t="s">
         <v>1464</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>1465</v>
-      </c>
-      <c r="D6" s="16" t="s">
-        <v>1466</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>552</v>
-      </c>
-      <c r="F6" s="15" t="s">
-        <v>649</v>
-      </c>
-      <c r="G6" s="15" t="s">
-        <v>484</v>
-      </c>
-      <c r="H6" s="15" t="s">
-        <v>485</v>
       </c>
     </row>
     <row r="7" spans="1:27">
@@ -31506,25 +31569,25 @@
         <v>77</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>651</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>1467</v>
+      </c>
+      <c r="H7" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>1467</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="8" spans="1:27">
@@ -31532,25 +31595,25 @@
         <v>75</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1468</v>
+      </c>
+      <c r="H8" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>1468</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>661</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="9" spans="1:27">
@@ -31558,25 +31621,25 @@
         <v>73</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>659</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>1469</v>
+      </c>
+      <c r="H9" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>1469</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="10" spans="1:27">
@@ -31584,25 +31647,25 @@
         <v>73</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>652</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>1470</v>
+      </c>
+      <c r="H10" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>1470</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>652</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H10" s="2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="11" spans="1:27">
@@ -31610,25 +31673,25 @@
         <v>80</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>655</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>1471</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>1471</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>655</v>
-      </c>
-      <c r="G11" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="12" spans="1:27">
@@ -31636,93 +31699,175 @@
         <v>78</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>653</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>488</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>1472</v>
+      </c>
+      <c r="H12" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>1472</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>653</v>
-      </c>
-      <c r="G12" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="H12" s="2" t="s">
-        <v>488</v>
       </c>
     </row>
     <row r="13" spans="1:27">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:27">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
     </row>
     <row r="15" spans="1:27" ht="11.25" customHeight="1">
-      <c r="A15" s="68" t="s">
+      <c r="A15" s="90" t="s">
+        <v>1582</v>
+      </c>
+      <c r="B15" s="122"/>
+      <c r="C15" s="122"/>
+      <c r="D15" s="90" t="s">
+        <v>1583</v>
+      </c>
+      <c r="E15" s="90"/>
+      <c r="F15" s="90" t="s">
+        <v>803</v>
+      </c>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:27" ht="11.25" customHeight="1">
+      <c r="A16" s="122"/>
+      <c r="B16" s="122"/>
+      <c r="C16" s="122"/>
+      <c r="D16" s="90"/>
+      <c r="E16" s="90"/>
+      <c r="F16" s="90"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="11.25" customHeight="1">
+      <c r="A17" s="122"/>
+      <c r="B17" s="122"/>
+      <c r="C17" s="122"/>
+      <c r="D17" s="90"/>
+      <c r="E17" s="90"/>
+      <c r="F17" s="90"/>
+    </row>
+    <row r="18" spans="1:8" ht="11.25" customHeight="1">
+      <c r="A18" s="68" t="s">
         <v>1473</v>
       </c>
-      <c r="B15" s="68"/>
-      <c r="C15" s="68" t="s">
+      <c r="B18" s="68" t="s">
         <v>585</v>
       </c>
-      <c r="D15" s="121" t="s">
+      <c r="C18" s="123" t="s">
+        <v>1475</v>
+      </c>
+      <c r="D18" s="88" t="s">
+        <v>1585</v>
+      </c>
+      <c r="E18" s="124" t="s">
+        <v>1584</v>
+      </c>
+      <c r="F18" s="68" t="s">
+        <v>491</v>
+      </c>
+      <c r="G18" s="121" t="s">
         <v>1581</v>
       </c>
-      <c r="E15" s="68" t="s">
-        <v>1475</v>
-      </c>
-      <c r="F15" s="68"/>
-      <c r="G15" s="68"/>
-      <c r="H15" s="68"/>
-    </row>
-    <row r="16" spans="1:27">
-      <c r="A16" s="68"/>
-      <c r="B16" s="68"/>
-      <c r="C16" s="68"/>
-      <c r="D16" s="121"/>
-      <c r="E16" s="68"/>
-      <c r="F16" s="68"/>
-      <c r="G16" s="68"/>
-      <c r="H16" s="68"/>
-    </row>
-    <row r="17" spans="1:8">
-      <c r="A17" s="68"/>
-      <c r="B17" s="68"/>
-      <c r="C17" s="68"/>
-      <c r="D17" s="121"/>
-      <c r="E17" s="68"/>
-      <c r="F17" s="68"/>
-      <c r="G17" s="68"/>
-      <c r="H17" s="68"/>
+      <c r="H18" s="68"/>
     </row>
     <row r="19" spans="1:8">
-      <c r="A19" s="120" t="s">
+      <c r="A19" s="68"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="123"/>
+      <c r="D19" s="88"/>
+      <c r="E19" s="124"/>
+      <c r="F19" s="68"/>
+      <c r="G19" s="121"/>
+      <c r="H19" s="68"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="123"/>
+      <c r="D20" s="88"/>
+      <c r="E20" s="124"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="121"/>
+      <c r="H20" s="68"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="D21" s="88"/>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="A22" s="120" t="s">
         <v>1474</v>
       </c>
-    </row>
-    <row r="20" spans="1:8">
-      <c r="A20" s="120"/>
+      <c r="D22" s="88"/>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="A23" s="120"/>
+      <c r="D23" s="88"/>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="D24" s="88"/>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="D25" s="88"/>
+    </row>
+    <row r="26" spans="1:8">
+      <c r="D26" s="88"/>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="D27" s="88"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="D28" s="88"/>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="D29" s="88"/>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="D30" s="88"/>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="D31" s="88"/>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="D32" s="88"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="14">
+    <mergeCell ref="C18:C20"/>
+    <mergeCell ref="E18:E20"/>
+    <mergeCell ref="F18:F20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="D18:D32"/>
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="B15:B17"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="E15:E17"/>
+    <mergeCell ref="A18:A20"/>
+    <mergeCell ref="H18:H20"/>
+    <mergeCell ref="B18:B20"/>
+    <mergeCell ref="A15:C17"/>
+    <mergeCell ref="D15:E17"/>
     <mergeCell ref="F15:F17"/>
-    <mergeCell ref="G15:G17"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="D15:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Mapeamento Conferência LN - DOM e PEC
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_DOM.xlsx
+++ b/Documentação/Planilhas/Conferencia_DOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="93" r:id="rId1"/>
@@ -85,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2916" uniqueCount="1595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2948" uniqueCount="1609">
   <si>
     <t>DESCR</t>
   </si>
@@ -4918,6 +4918,48 @@
   </si>
   <si>
     <t>stg_dom_tipo_operacao</t>
+  </si>
+  <si>
+    <t>CD_BANDEIRA_SITE</t>
+  </si>
+  <si>
+    <t>Pegar a informação da coluna Cód. Bandeira Site</t>
+  </si>
+  <si>
+    <t>38</t>
+  </si>
+  <si>
+    <t>50</t>
+  </si>
+  <si>
+    <t>37</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>42</t>
+  </si>
+  <si>
+    <t>49</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>Clube Extra</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>BNDES</t>
+  </si>
+  <si>
+    <t>51</t>
   </si>
 </sst>
 </file>
@@ -5600,18 +5642,6 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -5652,6 +5682,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7131,11 +7173,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B53" activePane="bottomRight" state="frozen"/>
+    <sheetView workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C63" sqref="C63"/>
+      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -14946,9 +14988,11 @@
   <sheetPr>
     <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AE97"/>
+  <dimension ref="A1:AE99"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -15010,6 +15054,9 @@
       <c r="B6" s="16" t="s">
         <v>230</v>
       </c>
+      <c r="C6" s="16" t="s">
+        <v>1595</v>
+      </c>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -15021,7 +15068,9 @@
       <c r="B7" s="7" t="s">
         <v>231</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="D7" s="6"/>
       <c r="E7" s="6"/>
       <c r="F7" s="6"/>
@@ -15034,6 +15083,9 @@
       <c r="B8" s="4" t="s">
         <v>232</v>
       </c>
+      <c r="C8" s="2" t="s">
+        <v>2</v>
+      </c>
       <c r="H8" s="1"/>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -15045,6 +15097,9 @@
       <c r="B9" s="4" t="s">
         <v>233</v>
       </c>
+      <c r="C9" s="2" t="s">
+        <v>3</v>
+      </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -15056,6 +15111,9 @@
       <c r="B10" s="4" t="s">
         <v>234</v>
       </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
@@ -15067,6 +15125,9 @@
       <c r="B11" s="4" t="s">
         <v>235</v>
       </c>
+      <c r="C11" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="H11" s="1"/>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
@@ -15078,6 +15139,9 @@
       <c r="B12" s="4" t="s">
         <v>236</v>
       </c>
+      <c r="C12" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
@@ -15089,6 +15153,9 @@
       <c r="B13" s="4" t="s">
         <v>385</v>
       </c>
+      <c r="C13" s="2" t="s">
+        <v>1597</v>
+      </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
@@ -15100,6 +15167,9 @@
       <c r="B14" s="4" t="s">
         <v>386</v>
       </c>
+      <c r="C14" s="2" t="s">
+        <v>14</v>
+      </c>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -15111,6 +15181,9 @@
       <c r="B15" s="4" t="s">
         <v>386</v>
       </c>
+      <c r="C15" s="2" t="s">
+        <v>1598</v>
+      </c>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
@@ -15122,6 +15195,9 @@
       <c r="B16" s="4" t="s">
         <v>387</v>
       </c>
+      <c r="C16" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
       <c r="J16" s="1"/>
@@ -15133,6 +15209,9 @@
       <c r="B17" s="4" t="s">
         <v>388</v>
       </c>
+      <c r="C17" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -15144,6 +15223,9 @@
       <c r="B18" s="4" t="s">
         <v>389</v>
       </c>
+      <c r="C18" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="J18" s="1"/>
@@ -15155,6 +15237,9 @@
       <c r="B19" s="4" t="s">
         <v>390</v>
       </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -15166,164 +15251,82 @@
       <c r="B20" s="4" t="s">
         <v>391</v>
       </c>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
     </row>
-    <row r="21" spans="1:30" s="2" customFormat="1">
+    <row r="21" spans="1:30">
       <c r="A21" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>392</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>1599</v>
       </c>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
-      <c r="Q21" s="1"/>
-      <c r="R21" s="1"/>
-      <c r="S21" s="1"/>
-      <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
-      <c r="V21" s="1"/>
-      <c r="W21" s="1"/>
-      <c r="X21" s="1"/>
-      <c r="Y21" s="1"/>
-      <c r="Z21" s="1"/>
-      <c r="AA21" s="1"/>
-      <c r="AB21" s="1"/>
-      <c r="AC21" s="1"/>
-      <c r="AD21" s="1"/>
-    </row>
-    <row r="22" spans="1:30" s="2" customFormat="1">
+    </row>
+    <row r="22" spans="1:30">
       <c r="A22" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>393</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>1600</v>
       </c>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
       <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
-      <c r="Q22" s="1"/>
-      <c r="R22" s="1"/>
-      <c r="S22" s="1"/>
-      <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
-      <c r="V22" s="1"/>
-      <c r="W22" s="1"/>
-      <c r="X22" s="1"/>
-      <c r="Y22" s="1"/>
-      <c r="Z22" s="1"/>
-      <c r="AA22" s="1"/>
-      <c r="AB22" s="1"/>
-      <c r="AC22" s="1"/>
-      <c r="AD22" s="1"/>
-    </row>
-    <row r="23" spans="1:30" s="2" customFormat="1">
+    </row>
+    <row r="23" spans="1:30">
       <c r="A23" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>394</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
       <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
-      <c r="Q23" s="1"/>
-      <c r="R23" s="1"/>
-      <c r="S23" s="1"/>
-      <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
-      <c r="V23" s="1"/>
-      <c r="W23" s="1"/>
-      <c r="X23" s="1"/>
-      <c r="Y23" s="1"/>
-      <c r="Z23" s="1"/>
-      <c r="AA23" s="1"/>
-      <c r="AB23" s="1"/>
-      <c r="AC23" s="1"/>
-      <c r="AD23" s="1"/>
-    </row>
-    <row r="24" spans="1:30" s="2" customFormat="1">
+    </row>
+    <row r="24" spans="1:30">
       <c r="A24" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>395</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
-      <c r="Q24" s="1"/>
-      <c r="R24" s="1"/>
-      <c r="S24" s="1"/>
-      <c r="T24" s="1"/>
-      <c r="U24" s="1"/>
-      <c r="V24" s="1"/>
-      <c r="W24" s="1"/>
-      <c r="X24" s="1"/>
-      <c r="Y24" s="1"/>
-      <c r="Z24" s="1"/>
-      <c r="AA24" s="1"/>
-      <c r="AB24" s="1"/>
-      <c r="AC24" s="1"/>
-      <c r="AD24" s="1"/>
-    </row>
-    <row r="25" spans="1:30" s="2" customFormat="1">
+    </row>
+    <row r="25" spans="1:30">
       <c r="A25" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>396</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>26</v>
       </c>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
       <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
-      <c r="Q25" s="1"/>
-      <c r="R25" s="1"/>
-      <c r="S25" s="1"/>
-      <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
-      <c r="V25" s="1"/>
-      <c r="W25" s="1"/>
-      <c r="X25" s="1"/>
-      <c r="Y25" s="1"/>
-      <c r="Z25" s="1"/>
-      <c r="AA25" s="1"/>
-      <c r="AB25" s="1"/>
-      <c r="AC25" s="1"/>
-      <c r="AD25" s="1"/>
     </row>
     <row r="26" spans="1:30" s="2" customFormat="1">
       <c r="A26" s="2" t="s">
@@ -15331,6 +15334,9 @@
       </c>
       <c r="B26" s="4" t="s">
         <v>397</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>1601</v>
       </c>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
@@ -15363,6 +15369,9 @@
       <c r="B27" s="4" t="s">
         <v>398</v>
       </c>
+      <c r="C27" s="2" t="s">
+        <v>1602</v>
+      </c>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
       <c r="J27" s="1"/>
@@ -15394,6 +15403,9 @@
       <c r="B28" s="4" t="s">
         <v>399</v>
       </c>
+      <c r="C28" s="2" t="s">
+        <v>506</v>
+      </c>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
       <c r="J28" s="1"/>
@@ -15418,120 +15430,227 @@
       <c r="AC28" s="1"/>
       <c r="AD28" s="1"/>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:30" s="2" customFormat="1">
       <c r="A29" s="2" t="s">
         <v>22</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>400</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>21</v>
       </c>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
-    </row>
-    <row r="30" spans="1:30">
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+      <c r="AB29" s="1"/>
+      <c r="AC29" s="1"/>
+      <c r="AD29" s="1"/>
+    </row>
+    <row r="30" spans="1:30" s="2" customFormat="1">
       <c r="A30" s="2" t="s">
         <v>23</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>401</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>1234</v>
       </c>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
-    </row>
-    <row r="31" spans="1:30">
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+      <c r="AB30" s="1"/>
+      <c r="AC30" s="1"/>
+      <c r="AD30" s="1"/>
+    </row>
+    <row r="31" spans="1:30" s="2" customFormat="1">
+      <c r="A31" s="2" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>1604</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>1605</v>
+      </c>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
-    </row>
-    <row r="32" spans="1:30" ht="22.5">
-      <c r="A32" s="18" t="s">
-        <v>403</v>
-      </c>
-      <c r="B32" s="18" t="s">
-        <v>404</v>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+      <c r="AB31" s="1"/>
+      <c r="AC31" s="1"/>
+      <c r="AD31" s="1"/>
+    </row>
+    <row r="32" spans="1:30" s="2" customFormat="1">
+      <c r="A32" s="2" t="s">
+        <v>1606</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>1607</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>1608</v>
       </c>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
-    </row>
-    <row r="33" spans="8:10">
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+      <c r="AB32" s="1"/>
+      <c r="AC32" s="1"/>
+      <c r="AD32" s="1"/>
+    </row>
+    <row r="33" spans="1:10">
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
       <c r="J33" s="1"/>
     </row>
-    <row r="34" spans="8:10">
+    <row r="34" spans="1:10" ht="22.5">
+      <c r="A34" s="18" t="s">
+        <v>403</v>
+      </c>
+      <c r="B34" s="18" t="s">
+        <v>404</v>
+      </c>
+      <c r="C34" s="18" t="s">
+        <v>1596</v>
+      </c>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
       <c r="J34" s="1"/>
     </row>
-    <row r="35" spans="8:10">
+    <row r="35" spans="1:10">
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
     </row>
-    <row r="36" spans="8:10">
+    <row r="36" spans="1:10">
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
       <c r="J36" s="1"/>
     </row>
-    <row r="37" spans="8:10">
+    <row r="37" spans="1:10">
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
       <c r="J37" s="1"/>
     </row>
-    <row r="38" spans="8:10">
+    <row r="38" spans="1:10">
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
       <c r="J38" s="1"/>
     </row>
-    <row r="39" spans="8:10">
+    <row r="39" spans="1:10">
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
       <c r="J39" s="1"/>
     </row>
-    <row r="40" spans="8:10">
+    <row r="40" spans="1:10">
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
       <c r="J40" s="1"/>
     </row>
-    <row r="41" spans="8:10">
+    <row r="41" spans="1:10">
       <c r="H41" s="1"/>
       <c r="I41" s="1"/>
       <c r="J41" s="1"/>
     </row>
-    <row r="42" spans="8:10">
+    <row r="42" spans="1:10">
       <c r="H42" s="1"/>
       <c r="I42" s="1"/>
       <c r="J42" s="1"/>
     </row>
-    <row r="43" spans="8:10">
+    <row r="43" spans="1:10">
       <c r="H43" s="1"/>
       <c r="I43" s="1"/>
       <c r="J43" s="1"/>
     </row>
-    <row r="44" spans="8:10">
+    <row r="44" spans="1:10">
       <c r="H44" s="1"/>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
     </row>
-    <row r="45" spans="8:10">
+    <row r="45" spans="1:10">
       <c r="H45" s="1"/>
       <c r="I45" s="1"/>
       <c r="J45" s="1"/>
     </row>
-    <row r="46" spans="8:10">
+    <row r="46" spans="1:10">
       <c r="H46" s="1"/>
       <c r="I46" s="1"/>
       <c r="J46" s="1"/>
     </row>
-    <row r="47" spans="8:10">
+    <row r="47" spans="1:10">
       <c r="H47" s="1"/>
       <c r="I47" s="1"/>
       <c r="J47" s="1"/>
     </row>
-    <row r="48" spans="8:10">
+    <row r="48" spans="1:10">
       <c r="H48" s="1"/>
       <c r="I48" s="1"/>
       <c r="J48" s="1"/>
@@ -15780,6 +15899,16 @@
       <c r="H97" s="1"/>
       <c r="I97" s="1"/>
       <c r="J97" s="1"/>
+    </row>
+    <row r="98" spans="8:10">
+      <c r="H98" s="1"/>
+      <c r="I98" s="1"/>
+      <c r="J98" s="1"/>
+    </row>
+    <row r="99" spans="8:10">
+      <c r="H99" s="1"/>
+      <c r="I99" s="1"/>
+      <c r="J99" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -16262,10 +16391,10 @@
       <c r="T17" s="2"/>
     </row>
     <row r="18" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A18" s="102" t="s">
+      <c r="A18" s="98" t="s">
         <v>849</v>
       </c>
-      <c r="B18" s="102" t="s">
+      <c r="B18" s="98" t="s">
         <v>850</v>
       </c>
       <c r="C18" s="2"/>
@@ -16274,16 +16403,16 @@
       <c r="W18" s="2"/>
     </row>
     <row r="19" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A19" s="103"/>
-      <c r="B19" s="103"/>
+      <c r="A19" s="99"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="2"/>
       <c r="J19" s="2"/>
       <c r="L19" s="2"/>
       <c r="W19" s="2"/>
     </row>
     <row r="20" spans="1:23" s="1" customFormat="1" ht="11.25" customHeight="1">
-      <c r="A20" s="103"/>
-      <c r="B20" s="103"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="2"/>
       <c r="J20" s="2"/>
       <c r="L20" s="2"/>
@@ -17053,53 +17182,53 @@
       <c r="M18" s="13"/>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1">
-      <c r="A19" s="104" t="s">
+      <c r="A19" s="100" t="s">
         <v>914</v>
       </c>
-      <c r="B19" s="110"/>
-      <c r="C19" s="110"/>
-      <c r="D19" s="110"/>
-      <c r="E19" s="110"/>
-      <c r="F19" s="110"/>
-      <c r="G19" s="110"/>
-      <c r="H19" s="107"/>
-      <c r="I19" s="104" t="s">
+      <c r="B19" s="106"/>
+      <c r="C19" s="106"/>
+      <c r="D19" s="106"/>
+      <c r="E19" s="106"/>
+      <c r="F19" s="106"/>
+      <c r="G19" s="106"/>
+      <c r="H19" s="103"/>
+      <c r="I19" s="100" t="s">
         <v>915</v>
       </c>
-      <c r="J19" s="107"/>
-      <c r="K19" s="104" t="s">
+      <c r="J19" s="103"/>
+      <c r="K19" s="100" t="s">
         <v>918</v>
       </c>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
     </row>
     <row r="20" spans="1:15" ht="11.25" customHeight="1">
-      <c r="A20" s="105"/>
-      <c r="B20" s="111"/>
-      <c r="C20" s="111"/>
-      <c r="D20" s="111"/>
-      <c r="E20" s="111"/>
-      <c r="F20" s="111"/>
-      <c r="G20" s="111"/>
-      <c r="H20" s="108"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="108"/>
-      <c r="K20" s="105"/>
+      <c r="A20" s="101"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="107"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="107"/>
+      <c r="H20" s="104"/>
+      <c r="I20" s="101"/>
+      <c r="J20" s="104"/>
+      <c r="K20" s="101"/>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
     </row>
     <row r="21" spans="1:15">
-      <c r="A21" s="106"/>
-      <c r="B21" s="112"/>
-      <c r="C21" s="112"/>
-      <c r="D21" s="112"/>
-      <c r="E21" s="112"/>
-      <c r="F21" s="112"/>
-      <c r="G21" s="112"/>
-      <c r="H21" s="109"/>
-      <c r="I21" s="106"/>
-      <c r="J21" s="109"/>
-      <c r="K21" s="106"/>
+      <c r="A21" s="102"/>
+      <c r="B21" s="108"/>
+      <c r="C21" s="108"/>
+      <c r="D21" s="108"/>
+      <c r="E21" s="108"/>
+      <c r="F21" s="108"/>
+      <c r="G21" s="108"/>
+      <c r="H21" s="105"/>
+      <c r="I21" s="102"/>
+      <c r="J21" s="105"/>
+      <c r="K21" s="102"/>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
     </row>
@@ -19157,8 +19286,8 @@
       <c r="A12" s="67" t="s">
         <v>1049</v>
       </c>
-      <c r="B12" s="113"/>
-      <c r="C12" s="113"/>
+      <c r="B12" s="109"/>
+      <c r="C12" s="109"/>
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
@@ -19183,8 +19312,8 @@
     </row>
     <row r="13" spans="1:33" s="2" customFormat="1">
       <c r="A13" s="67"/>
-      <c r="B13" s="113"/>
-      <c r="C13" s="113"/>
+      <c r="B13" s="109"/>
+      <c r="C13" s="109"/>
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
@@ -19209,8 +19338,8 @@
     </row>
     <row r="14" spans="1:33" s="2" customFormat="1">
       <c r="A14" s="67"/>
-      <c r="B14" s="113"/>
-      <c r="C14" s="113"/>
+      <c r="B14" s="109"/>
+      <c r="C14" s="109"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
@@ -19234,31 +19363,31 @@
       <c r="AG14" s="1"/>
     </row>
     <row r="16" spans="1:33">
-      <c r="A16" s="114" t="s">
+      <c r="A16" s="110" t="s">
         <v>1050</v>
       </c>
-      <c r="B16" s="115"/>
-      <c r="C16" s="115"/>
+      <c r="B16" s="111"/>
+      <c r="C16" s="111"/>
     </row>
     <row r="17" spans="1:3">
-      <c r="A17" s="115"/>
-      <c r="B17" s="115"/>
-      <c r="C17" s="115"/>
+      <c r="A17" s="111"/>
+      <c r="B17" s="111"/>
+      <c r="C17" s="111"/>
     </row>
     <row r="18" spans="1:3">
-      <c r="A18" s="115"/>
-      <c r="B18" s="115"/>
-      <c r="C18" s="115"/>
+      <c r="A18" s="111"/>
+      <c r="B18" s="111"/>
+      <c r="C18" s="111"/>
     </row>
     <row r="19" spans="1:3">
-      <c r="A19" s="115"/>
-      <c r="B19" s="115"/>
-      <c r="C19" s="115"/>
+      <c r="A19" s="111"/>
+      <c r="B19" s="111"/>
+      <c r="C19" s="111"/>
     </row>
     <row r="20" spans="1:3">
-      <c r="A20" s="115"/>
-      <c r="B20" s="115"/>
-      <c r="C20" s="115"/>
+      <c r="A20" s="111"/>
+      <c r="B20" s="111"/>
+      <c r="C20" s="111"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -21358,10 +21487,10 @@
       <c r="AF5" s="2"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1118</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="D6" s="36" t="s">
         <v>1114</v>
       </c>
@@ -21460,30 +21589,30 @@
       <c r="E15" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F15" s="98" t="s">
+      <c r="F15" s="114" t="s">
         <v>1120</v>
       </c>
     </row>
     <row r="16" spans="1:32">
       <c r="D16" s="68"/>
       <c r="E16" s="68"/>
-      <c r="F16" s="99"/>
+      <c r="F16" s="115"/>
     </row>
     <row r="19" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:6">
@@ -21500,10 +21629,10 @@
       <c r="F23" s="48"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="112" t="s">
         <v>1119</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="112"/>
       <c r="D25" s="36" t="s">
         <v>1114</v>
       </c>
@@ -21609,30 +21738,30 @@
       <c r="E36" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F36" s="98" t="s">
+      <c r="F36" s="114" t="s">
         <v>1121</v>
       </c>
     </row>
     <row r="37" spans="1:6">
       <c r="D37" s="68"/>
       <c r="E37" s="68"/>
-      <c r="F37" s="99"/>
+      <c r="F37" s="115"/>
     </row>
     <row r="38" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="113"/>
       <c r="C38" s="46"/>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="113"/>
       <c r="C39" s="46"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="113"/>
       <c r="C40" s="46"/>
     </row>
     <row r="41" spans="1:6">
@@ -21749,10 +21878,10 @@
       <c r="AF5" s="2"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1123</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="D6" s="36" t="s">
         <v>1127</v>
       </c>
@@ -21852,10 +21981,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>709</v>
@@ -21863,21 +21992,21 @@
       <c r="E19" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="114" t="s">
         <v>1124</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="99"/>
+      <c r="F20" s="115"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:6">
@@ -21894,10 +22023,10 @@
       <c r="F23" s="48"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="112" t="s">
         <v>1125</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="112"/>
       <c r="D25" s="36" t="s">
         <v>1127</v>
       </c>
@@ -22008,10 +22137,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="113"/>
       <c r="C38" s="46"/>
       <c r="D38" s="68" t="s">
         <v>709</v>
@@ -22019,21 +22148,21 @@
       <c r="E38" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F38" s="98" t="s">
+      <c r="F38" s="114" t="s">
         <v>1126</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="113"/>
       <c r="C39" s="46"/>
       <c r="D39" s="68"/>
       <c r="E39" s="68"/>
-      <c r="F39" s="99"/>
+      <c r="F39" s="115"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="113"/>
       <c r="C40" s="46"/>
     </row>
     <row r="41" spans="1:6">
@@ -22130,10 +22259,10 @@
       <c r="L3" s="13"/>
     </row>
     <row r="6" spans="1:33">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1138</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="36" t="s">
         <v>1135</v>
@@ -22309,10 +22438,10 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="1:7">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>709</v>
@@ -22320,23 +22449,23 @@
       <c r="E19" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="114" t="s">
         <v>1137</v>
       </c>
       <c r="G19" s="13"/>
     </row>
     <row r="20" spans="1:7">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="99"/>
+      <c r="F20" s="115"/>
       <c r="G20" s="13"/>
     </row>
     <row r="21" spans="1:7">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -22371,10 +22500,10 @@
       <c r="G24" s="13"/>
     </row>
     <row r="25" spans="1:7">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="112" t="s">
         <v>1139</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="112"/>
       <c r="C25" s="14"/>
       <c r="D25" s="36" t="s">
         <v>1135</v>
@@ -22556,10 +22685,10 @@
       <c r="G37" s="13"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="113"/>
       <c r="C38" s="46"/>
       <c r="D38" s="68" t="s">
         <v>709</v>
@@ -22567,23 +22696,23 @@
       <c r="E38" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F38" s="98" t="s">
+      <c r="F38" s="114" t="s">
         <v>1140</v>
       </c>
       <c r="G38" s="13"/>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="113"/>
       <c r="C39" s="46"/>
       <c r="D39" s="68"/>
       <c r="E39" s="68"/>
-      <c r="F39" s="99"/>
+      <c r="F39" s="115"/>
       <c r="G39" s="13"/>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="113"/>
       <c r="C40" s="46"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
@@ -22685,10 +22814,10 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1123</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="36" t="s">
         <v>1143</v>
@@ -22847,10 +22976,10 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>709</v>
@@ -22858,25 +22987,25 @@
       <c r="E19" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="114" t="s">
         <v>1124</v>
       </c>
       <c r="G19" s="13"/>
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="99"/>
+      <c r="F20" s="115"/>
       <c r="G20" s="13"/>
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="13"/>
       <c r="E21" s="13"/>
@@ -22915,10 +23044,10 @@
       <c r="L24" s="2"/>
     </row>
     <row r="25" spans="1:12">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="112" t="s">
         <v>1142</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="112"/>
       <c r="C25" s="14"/>
       <c r="D25" s="36" t="s">
         <v>1143</v>
@@ -23107,10 +23236,10 @@
       <c r="L37" s="2"/>
     </row>
     <row r="38" spans="1:12">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="113"/>
       <c r="C38" s="46"/>
       <c r="D38" s="68" t="s">
         <v>709</v>
@@ -23118,25 +23247,25 @@
       <c r="E38" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F38" s="98" t="s">
+      <c r="F38" s="114" t="s">
         <v>1141</v>
       </c>
       <c r="G38" s="13"/>
       <c r="L38" s="2"/>
     </row>
     <row r="39" spans="1:12">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="113"/>
       <c r="C39" s="46"/>
       <c r="D39" s="68"/>
       <c r="E39" s="68"/>
-      <c r="F39" s="99"/>
+      <c r="F39" s="115"/>
       <c r="G39" s="13"/>
       <c r="L39" s="2"/>
     </row>
     <row r="40" spans="1:12">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="113"/>
       <c r="C40" s="46"/>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
@@ -23257,10 +23386,10 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1156</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="19" t="s">
         <v>484</v>
@@ -23419,10 +23548,10 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>1157</v>
@@ -23437,8 +23566,8 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
@@ -23447,8 +23576,8 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
@@ -23549,10 +23678,10 @@
       <c r="L5" s="2"/>
     </row>
     <row r="6" spans="1:12">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1156</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="19" t="s">
         <v>1171</v>
@@ -23697,10 +23826,10 @@
       <c r="L18" s="2"/>
     </row>
     <row r="19" spans="1:12" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>1182</v>
@@ -23712,8 +23841,8 @@
       <c r="L19" s="2"/>
     </row>
     <row r="20" spans="1:12">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
@@ -23721,8 +23850,8 @@
       <c r="L20" s="2"/>
     </row>
     <row r="21" spans="1:12">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="68"/>
       <c r="E21" s="68"/>
@@ -25094,10 +25223,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1156</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1260</v>
@@ -25253,10 +25382,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1064</v>
@@ -25268,8 +25397,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -25277,8 +25406,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -26012,10 +26141,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1156</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1303</v>
@@ -26175,10 +26304,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1064</v>
@@ -26190,8 +26319,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -26199,8 +26328,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -28731,10 +28860,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1156</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1380</v>
@@ -28894,10 +29023,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1064</v>
@@ -28909,8 +29038,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -28918,8 +29047,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -29338,10 +29467,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1156</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>643</v>
@@ -29501,10 +29630,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1064</v>
@@ -29516,8 +29645,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -29525,8 +29654,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -29643,10 +29772,10 @@
       <c r="AF5" s="2"/>
     </row>
     <row r="6" spans="1:32">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1012</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="D6" s="36" t="s">
         <v>785</v>
       </c>
@@ -29768,10 +29897,10 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="68" t="s">
         <v>709</v>
@@ -29779,21 +29908,21 @@
       <c r="E19" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F19" s="98" t="s">
+      <c r="F19" s="114" t="s">
         <v>1013</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="68"/>
       <c r="E20" s="68"/>
-      <c r="F20" s="99"/>
+      <c r="F20" s="115"/>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
     </row>
     <row r="22" spans="1:6">
@@ -29810,10 +29939,10 @@
       <c r="F23" s="48"/>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="100" t="s">
+      <c r="A25" s="112" t="s">
         <v>1014</v>
       </c>
-      <c r="B25" s="100"/>
+      <c r="B25" s="112"/>
       <c r="D25" s="36" t="s">
         <v>785</v>
       </c>
@@ -29935,10 +30064,10 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="11.25" customHeight="1">
-      <c r="A38" s="101" t="s">
+      <c r="A38" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B38" s="101"/>
+      <c r="B38" s="113"/>
       <c r="C38" s="46"/>
       <c r="D38" s="68" t="s">
         <v>709</v>
@@ -29946,21 +30075,21 @@
       <c r="E38" s="68" t="s">
         <v>710</v>
       </c>
-      <c r="F38" s="98" t="s">
+      <c r="F38" s="114" t="s">
         <v>1017</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="101"/>
-      <c r="B39" s="101"/>
+      <c r="A39" s="113"/>
+      <c r="B39" s="113"/>
       <c r="C39" s="46"/>
       <c r="D39" s="68"/>
       <c r="E39" s="68"/>
-      <c r="F39" s="99"/>
+      <c r="F39" s="115"/>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="101"/>
-      <c r="B40" s="101"/>
+      <c r="A40" s="113"/>
+      <c r="B40" s="113"/>
       <c r="C40" s="46"/>
     </row>
     <row r="41" spans="1:6">
@@ -30053,10 +30182,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1156</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1403</v>
@@ -30216,10 +30345,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1064</v>
@@ -30231,8 +30360,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -30240,8 +30369,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>
@@ -30336,10 +30465,10 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11">
-      <c r="A6" s="100" t="s">
+      <c r="A6" s="112" t="s">
         <v>1156</v>
       </c>
-      <c r="B6" s="100"/>
+      <c r="B6" s="112"/>
       <c r="C6" s="14"/>
       <c r="D6" s="16" t="s">
         <v>1415</v>
@@ -30467,10 +30596,10 @@
       <c r="K18" s="2"/>
     </row>
     <row r="19" spans="1:11" ht="11.25" customHeight="1">
-      <c r="A19" s="101" t="s">
+      <c r="A19" s="113" t="s">
         <v>1584</v>
       </c>
-      <c r="B19" s="101"/>
+      <c r="B19" s="113"/>
       <c r="C19" s="46"/>
       <c r="D19" s="116" t="s">
         <v>1064</v>
@@ -30482,8 +30611,8 @@
       <c r="K19" s="2"/>
     </row>
     <row r="20" spans="1:11">
-      <c r="A20" s="101"/>
-      <c r="B20" s="101"/>
+      <c r="A20" s="113"/>
+      <c r="B20" s="113"/>
       <c r="C20" s="46"/>
       <c r="D20" s="117"/>
       <c r="E20" s="68"/>
@@ -30491,8 +30620,8 @@
       <c r="K20" s="2"/>
     </row>
     <row r="21" spans="1:11">
-      <c r="A21" s="101"/>
-      <c r="B21" s="101"/>
+      <c r="A21" s="113"/>
+      <c r="B21" s="113"/>
       <c r="C21" s="46"/>
       <c r="D21" s="118"/>
       <c r="E21" s="68"/>

</xml_diff>

<commit_message>
Atualização Documentação Conferência LN - DOM
</commit_message>
<xml_diff>
--- a/Documentação/Planilhas/Conferencia_DOM.xlsx
+++ b/Documentação/Planilhas/Conferencia_DOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="20115" windowHeight="7995" tabRatio="812" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Resumo" sheetId="93" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1317" uniqueCount="817">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1362" uniqueCount="845">
   <si>
     <t>DESCR</t>
   </si>
@@ -2529,6 +2529,90 @@
   </si>
   <si>
     <t>stg_dom_car_comando</t>
+  </si>
+  <si>
+    <t>CD_COMANDO</t>
+  </si>
+  <si>
+    <t>DS_COMANDO</t>
+  </si>
+  <si>
+    <t>TP_COMANDO</t>
+  </si>
+  <si>
+    <t>01</t>
+  </si>
+  <si>
+    <t>ENVIAR</t>
+  </si>
+  <si>
+    <t>02</t>
+  </si>
+  <si>
+    <t>Entrada confirmada</t>
+  </si>
+  <si>
+    <t>RETORNAR</t>
+  </si>
+  <si>
+    <t>Pedido de baixa</t>
+  </si>
+  <si>
+    <t>03</t>
+  </si>
+  <si>
+    <t>Entrada rejeitada ou instrução rejeitada</t>
+  </si>
+  <si>
+    <t>04</t>
+  </si>
+  <si>
+    <t>Concessão de abatimento</t>
+  </si>
+  <si>
+    <t>05</t>
+  </si>
+  <si>
+    <t>Cancelamento de abatimento</t>
+  </si>
+  <si>
+    <t>Liquidado sem Registro</t>
+  </si>
+  <si>
+    <t>06</t>
+  </si>
+  <si>
+    <t>Alteração de vencimento</t>
+  </si>
+  <si>
+    <t>Liquidação normal em dinheiro</t>
+  </si>
+  <si>
+    <t>07</t>
+  </si>
+  <si>
+    <t>Liquidação por conta em dinheiro</t>
+  </si>
+  <si>
+    <t>tfcmgl508m00l</t>
+  </si>
+  <si>
+    <t>Sessão tfcmgl508m00l (Códigos de Ocorrências) [filtro "Tipo Ocorrência" = Enviar]</t>
+  </si>
+  <si>
+    <t>Sessão tfcmgl508m00l (Códigos de Ocorrências) [filtro "Tipo Ocorrência" = Retornar]</t>
+  </si>
+  <si>
+    <t>Pegar a informação da coluna "Cód Ocorrência Interna"</t>
+  </si>
+  <si>
+    <t>Pegar a informação da coluna "Descrição Ocorrência"</t>
+  </si>
+  <si>
+    <t>Somente informações de ENVIAR</t>
+  </si>
+  <si>
+    <t>Somente informações de RETORNAR</t>
   </si>
 </sst>
 </file>
@@ -2632,7 +2716,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2678,6 +2762,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2946,7 +3036,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="106">
+  <cellXfs count="116">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3220,6 +3310,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="12" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -3229,11 +3325,35 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="5" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="6" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4030,7 +4150,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:C41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
@@ -12776,6 +12896,11 @@
     </row>
   </sheetData>
   <mergeCells count="12">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A38:B40"/>
+    <mergeCell ref="D38:D39"/>
+    <mergeCell ref="E38:E39"/>
+    <mergeCell ref="F38:F39"/>
     <mergeCell ref="E19:E20"/>
     <mergeCell ref="F19:F20"/>
     <mergeCell ref="A2:B2"/>
@@ -12783,11 +12908,6 @@
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A19:B21"/>
     <mergeCell ref="D19:D20"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A38:B40"/>
-    <mergeCell ref="D38:D39"/>
-    <mergeCell ref="E38:E39"/>
-    <mergeCell ref="F38:F39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14258,8 +14378,8 @@
       <c r="A15" s="79" t="s">
         <v>799</v>
       </c>
-      <c r="B15" s="101"/>
-      <c r="C15" s="101"/>
+      <c r="B15" s="103"/>
+      <c r="C15" s="103"/>
       <c r="D15" s="79" t="s">
         <v>800</v>
       </c>
@@ -14271,9 +14391,9 @@
       <c r="H15" s="2"/>
     </row>
     <row r="16" spans="1:27" ht="11.25" customHeight="1">
-      <c r="A16" s="101"/>
-      <c r="B16" s="101"/>
-      <c r="C16" s="101"/>
+      <c r="A16" s="103"/>
+      <c r="B16" s="103"/>
+      <c r="C16" s="103"/>
       <c r="D16" s="79"/>
       <c r="E16" s="79"/>
       <c r="F16" s="79"/>
@@ -14281,9 +14401,9 @@
       <c r="H16" s="2"/>
     </row>
     <row r="17" spans="1:8" ht="11.25" customHeight="1">
-      <c r="A17" s="101"/>
-      <c r="B17" s="101"/>
-      <c r="C17" s="101"/>
+      <c r="A17" s="103"/>
+      <c r="B17" s="103"/>
+      <c r="C17" s="103"/>
       <c r="D17" s="79"/>
       <c r="E17" s="79"/>
       <c r="F17" s="79"/>
@@ -14295,19 +14415,19 @@
       <c r="B18" s="58" t="s">
         <v>367</v>
       </c>
-      <c r="C18" s="102" t="s">
+      <c r="C18" s="104" t="s">
         <v>729</v>
       </c>
       <c r="D18" s="77" t="s">
         <v>802</v>
       </c>
-      <c r="E18" s="103" t="s">
+      <c r="E18" s="105" t="s">
         <v>801</v>
       </c>
       <c r="F18" s="58" t="s">
         <v>273</v>
       </c>
-      <c r="G18" s="105" t="s">
+      <c r="G18" s="102" t="s">
         <v>798</v>
       </c>
       <c r="H18" s="58"/>
@@ -14315,34 +14435,34 @@
     <row r="19" spans="1:8">
       <c r="A19" s="58"/>
       <c r="B19" s="58"/>
-      <c r="C19" s="102"/>
+      <c r="C19" s="104"/>
       <c r="D19" s="77"/>
-      <c r="E19" s="103"/>
+      <c r="E19" s="105"/>
       <c r="F19" s="58"/>
-      <c r="G19" s="105"/>
+      <c r="G19" s="102"/>
       <c r="H19" s="58"/>
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="58"/>
       <c r="B20" s="58"/>
-      <c r="C20" s="102"/>
+      <c r="C20" s="104"/>
       <c r="D20" s="77"/>
-      <c r="E20" s="103"/>
+      <c r="E20" s="105"/>
       <c r="F20" s="58"/>
-      <c r="G20" s="105"/>
+      <c r="G20" s="102"/>
       <c r="H20" s="58"/>
     </row>
     <row r="21" spans="1:8">
       <c r="D21" s="77"/>
     </row>
     <row r="22" spans="1:8">
-      <c r="A22" s="104" t="s">
+      <c r="A22" s="101" t="s">
         <v>728</v>
       </c>
       <c r="D22" s="77"/>
     </row>
     <row r="23" spans="1:8">
-      <c r="A23" s="104"/>
+      <c r="A23" s="101"/>
       <c r="D23" s="77"/>
     </row>
     <row r="24" spans="1:8">
@@ -14374,12 +14494,6 @@
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="G18:G20"/>
-    <mergeCell ref="D18:D32"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A18:A20"/>
     <mergeCell ref="H18:H20"/>
     <mergeCell ref="B18:B20"/>
     <mergeCell ref="A15:C17"/>
@@ -14388,6 +14502,12 @@
     <mergeCell ref="C18:C20"/>
     <mergeCell ref="E18:E20"/>
     <mergeCell ref="F18:F20"/>
+    <mergeCell ref="A22:A23"/>
+    <mergeCell ref="G18:G20"/>
+    <mergeCell ref="D18:D32"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A18:A20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -14401,7 +14521,9 @@
   </sheetPr>
   <dimension ref="A1:AG21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -14897,7 +15019,9 @@
   </sheetPr>
   <dimension ref="A1:AD28"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F32" sqref="F32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
@@ -15117,21 +15241,23 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr>
-    <tabColor rgb="FFFFFF00"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AD18"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.25"/>
   <cols>
-    <col min="1" max="1" width="21.7109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="21.5703125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="30.5703125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="17.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="18.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="2" customWidth="1"/>
+    <col min="1" max="1" width="18" style="2" customWidth="1"/>
+    <col min="2" max="2" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="28.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.7109375" style="2" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" style="2" customWidth="1"/>
     <col min="9" max="9" width="14.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20.5703125" style="1" customWidth="1"/>
@@ -15160,14 +15286,208 @@
         <v>493</v>
       </c>
       <c r="B3" s="54"/>
-      <c r="C3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>838</v>
+      </c>
       <c r="J3" s="2"/>
     </row>
     <row r="5" spans="1:30" ht="11.25" customHeight="1"/>
+    <row r="6" spans="1:30" ht="20.25" customHeight="1">
+      <c r="A6" s="106" t="s">
+        <v>817</v>
+      </c>
+      <c r="B6" s="106" t="s">
+        <v>818</v>
+      </c>
+      <c r="C6" s="106" t="s">
+        <v>819</v>
+      </c>
+      <c r="E6" s="106" t="s">
+        <v>817</v>
+      </c>
+      <c r="F6" s="106" t="s">
+        <v>818</v>
+      </c>
+      <c r="G6" s="106" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30">
+      <c r="A7" s="2" t="s">
+        <v>820</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>419</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>823</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30">
+      <c r="A8" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>825</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>826</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>827</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30">
+      <c r="A9" s="2" t="s">
+        <v>828</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>829</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>832</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30">
+      <c r="A10" s="2" t="s">
+        <v>830</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>831</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>835</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30">
+      <c r="A11" s="2" t="s">
+        <v>833</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>834</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>821</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>836</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>837</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>824</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30">
+      <c r="A13" s="107" t="s">
+        <v>839</v>
+      </c>
+      <c r="B13" s="108"/>
+      <c r="C13" s="109"/>
+      <c r="E13" s="107" t="s">
+        <v>840</v>
+      </c>
+      <c r="F13" s="108"/>
+      <c r="G13" s="109"/>
+    </row>
+    <row r="14" spans="1:30">
+      <c r="A14" s="110"/>
+      <c r="B14" s="111"/>
+      <c r="C14" s="112"/>
+      <c r="E14" s="110"/>
+      <c r="F14" s="111"/>
+      <c r="G14" s="112"/>
+    </row>
+    <row r="15" spans="1:30">
+      <c r="A15" s="113"/>
+      <c r="B15" s="114"/>
+      <c r="C15" s="115"/>
+      <c r="E15" s="113"/>
+      <c r="F15" s="114"/>
+      <c r="G15" s="115"/>
+    </row>
+    <row r="16" spans="1:30" ht="33.75" customHeight="1">
+      <c r="A16" s="58" t="s">
+        <v>841</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>842</v>
+      </c>
+      <c r="C16" s="58" t="s">
+        <v>843</v>
+      </c>
+      <c r="E16" s="58" t="s">
+        <v>841</v>
+      </c>
+      <c r="F16" s="58" t="s">
+        <v>842</v>
+      </c>
+      <c r="G16" s="58" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" s="58"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="58"/>
+      <c r="E17" s="58"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="58"/>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="58"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="58"/>
+      <c r="E18" s="58"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="58"/>
+    </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="10">
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A13:C15"/>
+    <mergeCell ref="E13:G15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="E16:E18"/>
+    <mergeCell ref="F16:F18"/>
+    <mergeCell ref="G16:G18"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>